<commit_message>
Begun formatting Testing Spreadsheet
To begin evaluating the effectiveness of our AI tool, we will be calculating F1 scores using pseudo-TP, FP, and FN measurements from the comparison of the AI responses against ground truths. These scores and gathered data will all be stored in the new ChatData.xlsx spreadsheet and used for further analysis later on.
</commit_message>
<xml_diff>
--- a/ChatData.xlsx
+++ b/ChatData.xlsx
@@ -1,52 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="Chat Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Chat Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,13 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,74 +444,278 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>User Prompt</v>
-      </c>
-      <c r="B1" t="str">
-        <v>AI Response</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>What monitor should I be buying?</v>
-      </c>
-      <c r="B2" t="str">
-        <v>"For gaming and esports, a high refresh rate monitor is essential for smooth gameplay and aiming precision. Aim for at least a 144Hz monitor, but ideally go for a 240Hz monitor for the best performance. Brands like ASUS, BenQ, and Alienware offer great options in terms of refresh rate, response time, and color accuracy. Make sure to also consider factors like panel type (TN, IPS, or VA) based on your preferences for color reproduction and viewing angles. Ultimately, prioritize a high refresh rate for a competitive edge in aiming and gameplay."</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>What aimers have played on 60hz?</v>
-      </c>
-      <c r="B3" t="str">
-        <v>"Players like eloevv and Mana have achieved impressive results in esports while using 60hz monitors. It goes to show that while having higher refresh rate monitors and top-notch equipment can be beneficial, it's not a strict requirement to excel in aiming and competitive gaming. Consistent practice, dedication, and skill are vital elements for success regardless of the hardware limitations."</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>What is the Bardoz Method or Bardpill meaning in static clicking in aim trainers?</v>
-      </c>
-      <c r="B4" t="str">
-        <v>"The Bardoz Method or Bardpill is a technique popularized in aim training communities, particularly in the context of static clicking scenarios. It involves utilizing a specific method of aiming that emphasizes consistency and precision. The Bardoz Method typically focuses on training the initial flick to each target to be fast, rigid, and explosive, while also incorporating smooth, narrow, and succinct micro corrections as needed. This technique aims to improve players' flicking abilities and overall accuracy in static clicking scenarios by honing both the initial flick and follow-up adjustments. It is named after its creator or popularizer in the community."</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>What static clicking scenarios are available in Kovaak's?</v>
-      </c>
-      <c r="B5" t="str">
-        <v>"In Kovaak's FPS Aim Trainer, some popular static clicking scenarios that focus on improving flicking techniques and high accuracy thresholds include 1wall6targets_small, 1wall4targets, 1wall3targets, ww3targets, Wide Wall 4 targets, Fourshot, and Threeshot. These scenarios help players familiarize themselves with basic flicking techniques by requiring them to quickly and accurately target stationary objects. By practicing these scenarios, players can develop the initial flick to each target to be fast, rigid, and explosive, while also honing their micro-correction skills to be smooth, narrow, and succinct."</v>
-      </c>
-    </row>
-    <row r="6" xml:space="preserve">
-      <c r="A6" t="str">
-        <v>What mouse should we be using in aim training?</v>
-      </c>
-      <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">"When it comes to choosing a mouse for aim training and esports, it's important to consider factors like sensor quality, DPI settings, weight, and shape. Popular options among professional players include models like the Logitech G Pro Wireless, Zowie EC2, and Finalmouse Ultralight 2. These mice are known for their precise sensors, lightweight design, and ergonomic shapes that cater to different grip styles.
-Ultimately, the best mouse for aim training is one that feels comfortable in your hand, offers customizable settings to suit your preferences, and provides accurate tracking for precise aiming. It's also beneficial to pair your mouse with a quality mousepad that complements your playstyle, whether you prefer a speed or control surface.
-Experimenting with different mice and"</v>
-      </c>
-    </row>
-    <row r="7" xml:space="preserve">
-      <c r="A7" t="str">
-        <v>Hello</v>
-      </c>
-      <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">Internal Server Error - Issue processing the request. Generated Chunk: 
-            No matching chunk found.</v>
-      </c>
-    </row>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>User Prompt</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>AI Response</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Generated Chunk</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ground Truth</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>What monitor should I be buying?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>"For gaming and esports, a high refresh rate monitor is essential for smooth gameplay and aiming precision. Aim for at least a 144Hz monitor, but ideally go for a 240Hz monitor for the best performance. Brands like ASUS, BenQ, and Alienware offer great options in terms of refresh rate, response time, and color accuracy. Make sure to also consider factors like panel type (TN, IPS, or VA) based on your preferences for color reproduction and viewing angles. Ultimately, prioritize a high refresh rate for a competitive edge in aiming and gameplay."</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Get at least a 144hz monitor, ideally 240hz. Get a modern gaming mouse with a good sensor and a low maintenance mousepad with a speed appropriate for you. Upgrade your PC specs. Maybe experiment with mouse skates or a gaming sleeve. Even if you are discouraged about your setup and do not want to spend a fortune, keep in mind that some very top level aimers have achieved great things on 60hz monitors. Specifically, players like eloevv and Mana.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>For competitive gaming and esports, a high refresh rate monitor is preferred for smooth gameplay and strong aiming performance. Try to get at least 144hz if you take things seriously, although 240hz is the ideal. More serious aimers may even go to 360hz monitors. Also, you may want to consider looking into different panels, like TN, IPS, or OLED, based on your desired motion clarity and color vibrance. Such factors can be a competitive advantage.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>What aimers have played on 60hz?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"Players like eloevv and Mana have achieved impressive results in esports while using 60hz monitors. It goes to show that while having higher refresh rate monitors and top-notch equipment can be beneficial, it's not a strict requirement to excel in aiming and competitive gaming. Consistent practice, dedication, and skill are vital elements for success regardless of the hardware limitations."</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Get at least a 144hz monitor, ideally 240hz. Get a modern gaming mouse with a good sensor and a low maintenance mousepad with a speed appropriate for you. Upgrade your PC specs. Maybe experiment with mouse skates or a gaming sleeve. Even if you are discouraged about your setup and do not want to spend a fortune, keep in mind that some very top level aimers have achieved great things on 60hz monitors. Specifically, players like eloevv and Mana.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Many aimers have likely played or started by playing on 60hz, but upgraded in the future. Famously, eloevv and Mana are two aimers that have consistently performed on 60hz, achieving tracking and dynamic scores in the Nova ranks. This simply goes to show how far dedication and focused practice can take you, even without the ideal gear.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>What is the Bardoz Method or Bardpill meaning in static clicking in aim trainers?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"The Bardoz Method or Bardpill is a technique popularized in aim training communities, particularly in the context of static clicking scenarios. It involves utilizing a specific method of aiming that emphasizes consistency and precision. The Bardoz Method typically focuses on training the initial flick to each target to be fast, rigid, and explosive, while also incorporating smooth, narrow, and succinct micro corrections as needed. This technique aims to improve players' flicking abilities and overall accuracy in static clicking scenarios by honing both the initial flick and follow-up adjustments. It is named after its creator or popularizer in the community."</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>This baseline process of initial flick into micro correction into shot confirmation is known as the Bardoz Method, coined after the former best static clicking player, Bardoz. The Bardoz Method, when performed correctly, is the current best way to maximize static clicking scenario scores and is a foundational technique for all forms of flicking-oriented aiming. The initial flick is usually expected to land at some offset difference before the target, the micro correction corrects this offset, and the shot confirmation is a brief visual check to ensure that you will land your shot. The method encourages high accuracy.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Bardoz and Bardpill methods are used in static clicking aim training scenarios. It emphasizes consistency and accuracy over raw speed. The Bardoz Method typically focuses on training the initial flick to each target to be fast, rigid, and explosive, while also incorporating smooth, narrow, and succinct micro corrections as needed. This technique aims to improve players' flicking abilities and overall accuracy in static clicking scenarios by honing both the initial flick and follow-up adjustments. It is named after its creator, Bardoz, one of the greatest players in static clicking history.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>What static clicking scenarios are available in Kovaak's?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"In Kovaak's FPS Aim Trainer, some popular static clicking scenarios that focus on improving flicking techniques and high accuracy thresholds include 1wall6targets_small, 1wall4targets, 1wall3targets, ww3targets, Wide Wall 4 targets, Fourshot, and Threeshot. These scenarios help players familiarize themselves with basic flicking techniques by requiring them to quickly and accurately target stationary objects. By practicing these scenarios, players can develop the initial flick to each target to be fast, rigid, and explosive, while also honing their micro-correction skills to be smooth, narrow, and succinct."</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Static clicking is the first subcategory of Clicking. All targets in these scenarios are stationary. The goal of most static clicking scenarios is to help players famliarize themselves with basic flicking techniques. Players should expect to hit high accuracy thresholds, upwards of 90-92%. Static clicking scenario examples include 1w6ts (1wall6targets_small), 1w4ts, 1w3ts, ww3t, Wide Wall 4 targets, Fourshot, Threeshot, and other similarly named scenarios. Static clicking places a focus on the initial flick to each target, which should be fast, rigid, and explosive, versus the micro correction, which needs to be smooth, narrow, and succinct.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>What mouse should we be using in aim training?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>"When it comes to choosing a mouse for aim training and esports, it's important to consider factors like sensor quality, DPI settings, weight, and shape. Popular options among professional players include models like the Logitech G Pro Wireless, Zowie EC2, and Finalmouse Ultralight 2. These mice are known for their precise sensors, lightweight design, and ergonomic shapes that cater to different grip styles._x000D_
+_x000D_
+Ultimately, the best mouse for aim training is one that feels comfortable in your hand, offers customizable settings to suit your preferences, and provides accurate tracking for precise aiming. It's also beneficial to pair your mouse with a quality mousepad that complements your playstyle, whether you prefer a speed or control surface._x000D_
+_x000D_
+Experimenting with different mice and"</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Get at least a 144hz monitor, ideally 240hz. Get a modern gaming mouse with a good sensor and a low maintenance mousepad with a speed appropriate for you. Upgrade your PC specs. Maybe experiment with mouse skates or a gaming sleeve. Even if you are discouraged about your setup and do not want to spend a fortune, keep in mind that some very top level aimers have achieved great things on 60hz monitors. Specifically, players like eloevv and Mana.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>What monitors are available that are best for FPS?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>"For FPS gaming, it's recommended to look for monitors with high refresh rates like 144Hz or ideally 240Hz for the smoothest gameplay experience. Some popular options among professional FPS players include monitors from brands like ASUS, BenQ, Alienware, and Zowie. Models such as the ASUS ROG Swift PG258Q, BenQ Zowie XL2540, Alienware AW2518H, and Zowie XL2546 are commonly praised for their fast response times and smooth performance in FPS games. Be sure to also consider factors like panel type (TN for faster response or IPS for better colors), resolution, and input lag when choosing the best monitor for your FPS gaming needs."</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Get at least a 144hz monitor, ideally 240hz. Get a modern gaming mouse with a good sensor and a low maintenance mousepad with a speed appropriate for you. Upgrade your PC specs. Maybe experiment with mouse skates or a gaming sleeve. Even if you are discouraged about your setup and do not want to spend a fortune, keep in mind that some very top level aimers have achieved great things on 60hz monitors. Specifically, players like eloevv and Mana.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>What aim training software is the best?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>"There are several popular aim training software options that many gamers and esports professionals use to improve their aiming skills. Some of the most well-known programs include Aim Lab, Kovaak's FPS Aim Trainer, and Aimtastic. These platforms offer various exercises and scenarios to help players enhance their aiming abilities through consistent practice and feedback. Ultimately, the best aim training software for you may depend on your personal preferences, the games you play, and the specific skills you want to focus on improving. It's recommended to try out different programs to see which one aligns best with your training goals and playstyle."</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Muscle memory is a misnomer in aiming. The term “muscle memory” when used improperly suggests that you should stick to a specific sensitivity across all situations to preserve consistency, and changing your sensitivity would ruin your muscle memory. This is a very simplified and inaccurate understanding of motor memory, an important idea in neuroscience. Because aiming has little to no formal research, it is best not to worry about muscle/motor memory, even when discussed as a proper neuroscience concept, as its role in aiming is not well understood.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Why is muscle memory considered a misnomer in aiming?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>"Muscle memory is often associated with repetitive movements that become automatic over time. While aim training can help improve muscle memory for precise aiming, it is a bit of a misnomer when it comes to aiming in esports. Aiming in gaming involves dynamic situations with constantly changing variables such as movement, positioning, and decision-making, rather than just repeating the same physical motion. Therefore, while muscle memory can contribute to more consistent aiming, it is not the only factor in mastering aiming skills in esports, where game sense, positioning, and decision-making play crucial roles."</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>The aim trainer will not help you have better positioning in game or stronger game sense that would influence decision-making skills. Essentially, aim training will NOT help you to improve at anything that can be considered a part of game-specific knowledge or mechanics that are not aim-related.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>What aim training should I be doing for Overwatch?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>"For Overwatch, aim training should focus on a combination of tracking and flick shots, as the game requires a mix of both skills depending on the hero you are playing. Here are some aim training routines that can benefit Overwatch players:
+1. **Tracking Aim**: Use aim training scenarios that involve tracking moving targets smoothly. This will help improve your aim with heroes like Soldier: 76, Zarya, and Tracer.
+2. **Flick Aim**: Practice scenarios that require quick and precise flick shots to improve your aim with heroes like Widowmaker, McCree, and Ana.
+3. **Vertical Aim**: Since Overwatch has a lot of verticality, practice aiming both horizontally and vertically to be able to track and hit targets in all dimensions.
+4."</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>“What sensitivity should I use? ” is probably the most frequently asked question by beginners. By and large, most people will say that sensitivity is up to preference, but most people use somewhere between 20cm/360° to 50cm/360°. This is not a hard rule, but most people’s ideal sensitivity lands within that range. Typically, you should prefer slower sensitivities for games that are more “flick” reliant, like CSGO or Valorant, and higher sensitivities for games that require more tracking or verticality, such as Overwatch or Fortnite. Feel free to experiment with different sensitivities often and find what works for you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>What is the optimal sensitivity for aiming?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>"The optimal sensitivity for aiming varies from player to player based on personal preference, playstyle, and the game being played. As mentioned in the text, most players tend to use sensitivities ranging from 20cm/360� to 50cm/360�. However, the key is to find a sensitivity that allows you to be accurate and consistent in your aiming. 
+For games that require precise flick shots like CSGO or Valorant, lower sensitivities are generally preferred as they offer more control. On the other hand, games that require quick tracking and vertical aiming like Overwatch or Fortnite might benefit from slightly higher sensitivities to allow for faster movements.
+It's essential to experiment with different sensitivities to find what feels comfortable and effective for you"</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>“What sensitivity should I use? ” is probably the most frequently asked question by beginners. By and large, most people will say that sensitivity is up to preference, but most people use somewhere between 20cm/360° to 50cm/360°. This is not a hard rule, but most people’s ideal sensitivity lands within that range. Typically, you should prefer slower sensitivities for games that are more “flick” reliant, like CSGO or Valorant, and higher sensitivities for games that require more tracking or verticality, such as Overwatch or Fortnite. Feel free to experiment with different sensitivities often and find what works for you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>What is static clicking meant to train for?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>"Static clicking scenarios are designed to train players in developing their basic flicking techniques and improving their accuracy. These scenarios help players familiarize themselves with the initial flick to each stationary target, emphasizing speed, precision, and explosiveness. By hitting high accuracy thresholds, players can enhance their ability to quickly and accurately flick to targets in a controlled and efficient manner. Static clicking also helps in honing the balance between fast initial movements and smooth micro corrections, which are crucial skills for various esports games that require precise aim and quick reactions."</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Static clicking is the first subcategory of Clicking. All targets in these scenarios are stationary. The goal of most static clicking scenarios is to help players famliarize themselves with basic flicking techniques. Players should expect to hit high accuracy thresholds, upwards of 90-92%. Static clicking scenario examples include 1w6ts (1wall6targets_small), 1w4ts, 1w3ts, ww3t, Wide Wall 4 targets, Fourshot, Threeshot, and other similarly named scenarios. Static clicking places a focus on the initial flick to each target, which should be fast, rigid, and explosive, versus the micro correction, which needs to be smooth, narrow, and succinct.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Continued Adding to Testing data and Fixed promptKeywords bug
Fixed a bug in promptKeywords that saw FAQ strings not being considered correctly in finding the appropriate chunk for the user prompt. Continued adding to the ChatData testing sheet. Tested various community-submitted user prompts.
</commit_message>
<xml_diff>
--- a/ChatData.xlsx
+++ b/ChatData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -489,10 +489,10 @@
         <v>What mouse should we be using in aim training?</v>
       </c>
       <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">"When it comes to choosing a mouse for aim training and esports, it&amp;apos;s important to consider factors like sensor quality, DPI settings, weight, and shape. Popular options among professional players include models like the Logitech G Pro Wireless, Zowie EC2, and Finalmouse Ultralight 2. These mice are known for their precise sensors, lightweight design, and ergonomic shapes that cater to different grip styles._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Ultimately, the best mouse for aim training is one that feels comfortable in your hand, offers customizable settings to suit your preferences, and provides accurate tracking for precise aiming. It&amp;apos;s also beneficial to pair your mouse with a quality mousepad that complements your playstyle, whether you prefer a speed or control surface._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">"When it comes to choosing a mouse for aim training and esports, it&amp;apos;s important to consider factors like sensor quality, DPI settings, weight, and shape. Popular options among professional players include models like the Logitech G Pro Wireless, Zowie EC2, and Finalmouse Ultralight 2. These mice are known for their precise sensors, lightweight design, and ergonomic shapes that cater to different grip styles._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Ultimately, the best mouse for aim training is one that feels comfortable in your hand, offers customizable settings to suit your preferences, and provides accurate tracking for precise aiming. It&amp;apos;s also beneficial to pair your mouse with a quality mousepad that complements your playstyle, whether you prefer a speed or control surface._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Experimenting with different mice and"</v>
       </c>
       <c r="C6" t="str">
@@ -549,14 +549,14 @@
         <v>What aim training should I be doing for Overwatch?</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">"For Overwatch, aim training should focus on a combination of tracking and flick shots, as the game requires a mix of both skills depending on the hero you are playing. Here are some aim training routines that can benefit Overwatch players:_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-1. **Tracking Aim**: Use aim training scenarios that involve tracking moving targets smoothly. This will help improve your aim with heroes like Soldier: 76, Zarya, and Tracer._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-2. **Flick Aim**: Practice scenarios that require quick and precise flick shots to improve your aim with heroes like Widowmaker, McCree, and Ana._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-3. **Vertical Aim**: Since Overwatch has a lot of verticality, practice aiming both horizontally and vertically to be able to track and hit targets in all dimensions._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">"For Overwatch, aim training should focus on a combination of tracking and flick shots, as the game requires a mix of both skills depending on the hero you are playing. Here are some aim training routines that can benefit Overwatch players:_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+1. **Tracking Aim**: Use aim training scenarios that involve tracking moving targets smoothly. This will help improve your aim with heroes like Soldier: 76, Zarya, and Tracer._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+2. **Flick Aim**: Practice scenarios that require quick and precise flick shots to improve your aim with heroes like Widowmaker, McCree, and Ana._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+3. **Vertical Aim**: Since Overwatch has a lot of verticality, practice aiming both horizontally and vertically to be able to track and hit targets in all dimensions._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 4."</v>
       </c>
       <c r="C10" t="str">
@@ -571,10 +571,10 @@
         <v>What is the optimal sensitivity for aiming?</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">"The optimal sensitivity for aiming varies from player to player based on personal preference, playstyle, and the game being played. As mentioned in the text, most players tend to use sensitivities ranging from 20cm/360� to 50cm/360�. However, the key is to find a sensitivity that allows you to be accurate and consistent in your aiming. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-For games that require precise flick shots like CSGO or Valorant, lower sensitivities are generally preferred as they offer more control. On the other hand, games that require quick tracking and vertical aiming like Overwatch or Fortnite might benefit from slightly higher sensitivities to allow for faster movements._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">"The optimal sensitivity for aiming varies from player to player based on personal preference, playstyle, and the game being played. As mentioned in the text, most players tend to use sensitivities ranging from 20cm/360� to 50cm/360�. However, the key is to find a sensitivity that allows you to be accurate and consistent in your aiming. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+For games that require precise flick shots like CSGO or Valorant, lower sensitivities are generally preferred as they offer more control. On the other hand, games that require quick tracking and vertical aiming like Overwatch or Fortnite might benefit from slightly higher sensitivities to allow for faster movements._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 It&amp;apos;s essential to experiment with different sensitivities to find what feels comfortable and effective for you"</v>
       </c>
       <c r="C11" t="str">
@@ -622,8 +622,8 @@
         <v>What do I exercise for my wrist health?</v>
       </c>
       <c r="B15" t="str" xml:space="preserve">
-        <v xml:space="preserve">"For wrist health, it is important to focus on strengthening exercises to prevent injuries such as tendinopathy, which is common among FPS esports players. You can start by doing wrist flexor weight-lifting exercises with dumbbells to build endurance and strength in your wrist muscles and tendons. Additionally, incorporating exercises that target wrist extension and rotation can help improve overall wrist mobility and stability._x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">"For wrist health, it is important to focus on strengthening exercises to prevent injuries such as tendinopathy, which is common among FPS esports players. You can start by doing wrist flexor weight-lifting exercises with dumbbells to build endurance and strength in your wrist muscles and tendons. Additionally, incorporating exercises that target wrist extension and rotation can help improve overall wrist mobility and stability._x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
 It is essential to gradually increase the intensity and duration of your exercises to avoid overloading your wrists. Remember that consistency is key, and it may take several weeks of consistent training to see improvements in muscle strength and endurance. However, if you experience sharp or concerning pain during or after exercising, it is important to stop and consult with a healthcare professional to avoid exacerbating"</v>
       </c>
     </row>
@@ -640,14 +640,14 @@
         <v>Why is it that some people improve at a much faster rate than others?</v>
       </c>
       <c r="B17" t="str" xml:space="preserve">
-        <v xml:space="preserve">"There are several factors that can contribute to why some people improve at a faster rate than others in esports or aim training. Some of these factors include:_x000d__x000d_
-_x000d__x000d_
-1. **Natural Talent**: Some individuals may have a natural aptitude for certain games or aiming skills, giving them an initial advantage when starting out._x000d__x000d_
-_x000d__x000d_
-2. **Experience**: Prior experience with gaming or similar activities can give players a head start in terms of understanding game mechanics, strategy, and developing hand-eye coordination._x000d__x000d_
-_x000d__x000d_
-3. **Practice Habits**: Consistent and focused practice can greatly accelerate skill development. Those who dedicate more time to deliberate practice tend to improve faster._x000d__x000d_
-_x000d__x000d_
+        <v xml:space="preserve">"There are several factors that can contribute to why some people improve at a faster rate than others in esports or aim training. Some of these factors include:_x000d__x000d__x000d_
+_x000d__x000d__x000d_
+1. **Natural Talent**: Some individuals may have a natural aptitude for certain games or aiming skills, giving them an initial advantage when starting out._x000d__x000d__x000d_
+_x000d__x000d__x000d_
+2. **Experience**: Prior experience with gaming or similar activities can give players a head start in terms of understanding game mechanics, strategy, and developing hand-eye coordination._x000d__x000d__x000d_
+_x000d__x000d__x000d_
+3. **Practice Habits**: Consistent and focused practice can greatly accelerate skill development. Those who dedicate more time to deliberate practice tend to improve faster._x000d__x000d__x000d_
+_x000d__x000d__x000d_
 4. **Mental Attitude**: A positive mindset, resilience in the face of setbacks, and a willingness to learn from mistakes"</v>
       </c>
     </row>
@@ -656,7 +656,8 @@
         <v>What is edge tracking, and where is edge tracking used the most?</v>
       </c>
       <c r="B18" t="str" xml:space="preserve">
-        <v xml:space="preserve">"Edge tracking is a technique used in aim training to improve precision and control by deliberately underaiming the target. By withholding tension in the wrist and performing a smoother reaction, edge tracking allows the player to have a bit more time on target, leading to more accurate shots. This technique is particularly useful in scenarios that involve reactive tracking, where quick yet controlled reactions are necessary to hit fast-moving targets.
+        <v xml:space="preserve">"Edge tracking is a technique used in aim training to improve precision and control by deliberately underaiming the target. By withholding tension in the wrist and performing a smoother reaction, edge tracking allows the player to have a bit more time on target, leading to more accurate shots. This technique is particularly useful in scenarios that involve reactive tracking, where quick yet controlled reactions are necessary to hit fast-moving targets._x000d_
+_x000d_
 Edge tracking is commonly used in aim training scenarios that focus on improving reactive tracking skills, such as in scenarios like Air, Ground Plaza, and Fuglaa variants in aim training platforms like Kovaak&amp;apos;s. These scenarios require players to react swiftly to moving targets while maintaining smoothness and stability in their aim adjustments. By incorporating edge tracking into their practice"</v>
       </c>
     </row>
@@ -665,16 +666,156 @@
         <v>How do I trust and commit to target direction changes?</v>
       </c>
       <c r="B19" t="str" xml:space="preserve">
-        <v xml:space="preserve">"Trusting and committing to target direction changes in target switching requires a combination of prediction, practice, and muscle memory. Here are some tips to help you improve in this area:
-1. **Prediction and Anticipation**: By understanding movement patterns and anticipating where the target is likely to go next, you can preemptively adjust your aim in that direction. This will help you to trust your initial flick and commit to following through with your tracking motion.
-2. **Practice and Repetition**: Consistent practice in scenarios that involve target switching will help you build muscle memory and improve your ability to trust your aim. The more you practice, the more confident you will become in your ability to hit moving targets.
+        <v xml:space="preserve">"Trusting and committing to target direction changes in target switching requires a combination of prediction, practice, and muscle memory. Here are some tips to help you improve in this area:_x000d_
+_x000d_
+1. **Prediction and Anticipation**: By understanding movement patterns and anticipating where the target is likely to go next, you can preemptively adjust your aim in that direction. This will help you to trust your initial flick and commit to following through with your tracking motion._x000d_
+_x000d_
+2. **Practice and Repetition**: Consistent practice in scenarios that involve target switching will help you build muscle memory and improve your ability to trust your aim. The more you practice, the more confident you will become in your ability to hit moving targets._x000d_
+_x000d_
 3. **Focus on Initial Flick Accuracy**:"</v>
+      </c>
+    </row>
+    <row r="20" xml:space="preserve">
+      <c r="A20" t="str">
+        <v>How do I fix overreactive habits and overreacting in general in tracking aim?</v>
+      </c>
+      <c r="B20" t="str" xml:space="preserve">
+        <v xml:space="preserve">"To address overreactive habits and improve tracking aim, it&amp;apos;s important to focus on developing better control and smoothness in your movements. Here are some tips to help you fix overreacting in tracking aim:
+1. **Practice Smooth Tracking**: Focus on tracking your target smoothly and predictively rather than reacting impulsively. Train yourself to follow the target&amp;apos;s movement methodically without jerky or sudden corrections.
+2. **Sensitivity Adjustment**: Consider adjusting your sensitivity settings to find a balance between being able to track smoothly and react quickly when needed. Experiment with different sensitivity levels to see what works best for you.
+3. **Crosshair Placement**: Pay attention to your crosshair placement and keep it close to the target while tracking. This will help reduce"</v>
+      </c>
+    </row>
+    <row r="21" xml:space="preserve">
+      <c r="A21" t="str">
+        <v>What mouse, mousepad, and skate combos work well or speed up improvement?</v>
+      </c>
+      <c r="B21" t="str" xml:space="preserve">
+        <v xml:space="preserve">"To enhance your tracking performance and speed up improvement, using the right mouse, mousepad, and skate combinations can make a significant difference. Here are some recommendations based on their impact on tracking aim:
+1. **Mouse**: 
+   - Look for a mouse that fits comfortably in your hand and allows for smooth and precise movements. Consider mice with a high-quality sensor for accurate tracking. Popular options for tracking include the Logitech G Pro Wireless, Zowie EC2 series, and Razer DeathAdder Elite.
+2. **Mousepad**:
+   - A good mousepad can provide a consistent surface for your mouse to glide on, crucial for maintaining smooth tracking. Opt for a larger mousepad to give yourself more space to move your mouse comfortably"</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Is there an optimal sensitivity to use for all games?</v>
+      </c>
+      <c r="B22" t="str">
+        <v>"There isn&amp;apos;t a one-size-fits-all optimal sensitivity for all games because the ideal sensitivity can vary based on individual preferences, playstyle, and the specific game being played. In general, a sensitivity that allows for precise aiming while still being comfortable and controllable is considered optimal. Players often experiment with different sensitivities to find what works best for them, and then practice to build muscle memory with that sensitivity. It&amp;apos;s important to find a sensitivity that provides a good balance between being able to make quick turns and precise adjustments. Remember that consistency and comfort are key factors when choosing a sensitivity that works well for you across different games."</v>
+      </c>
+    </row>
+    <row r="23" xml:space="preserve">
+      <c r="A23" t="str">
+        <v>Why is it so hard to make micro adjustments?</v>
+      </c>
+      <c r="B23" t="str" xml:space="preserve">
+        <v xml:space="preserve">"Making precise micro adjustments in tracking can be challenging due to the intricate balance required between maintaining a steady hand to keep the crosshair on target and making small adjustments to correct your aim. Factors such as muscle tension, hand-eye coordination, and reaction speed all play a role in executing successful micro adjustments. 
+Moreover, the pressure to react quickly in fast-paced games or scenarios can lead to overcompensating or underestimating the amount of correction needed. It requires a high level of focus, control, and practice to consistently make accurate micro adjustments without introducing shakiness or inconsistency in your aim.
+To improve your ability to make micro adjustments effectively, it is crucial to work on developing muscle memory, refining your sensitivity settings, and practicing regularly in scenarios that"</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>What areas of my hand or arm do I need to tense up more to make micro corrections?</v>
+      </c>
+      <c r="B24" t="str">
+        <v>"To make micro corrections in static clicking scenarios, you should focus on tensing up your fingers and wrist more than your entire arm. When making these precise adjustments to fine-tune your aim, it&amp;apos;s crucial to keep your arm and shoulder muscles relaxed to allow for smooth and controlled movements. By focusing on tensing up your fingers and wrist, you can make subtle adjustments without sacrificing speed or accuracy. Remember to keep the rest of your arm loose and maintain a fluid motion to achieve optimal performance in static clicking scenarios."</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>What is the perfect sensitivity for any game?</v>
+      </c>
+      <c r="B25" t="str">
+        <v>"The perfect sensitivity for any game varies from player to player as it depends on personal preference, playstyle, and physical capabilities. However, a common guideline is to find a sensitivity that allows you to make precise aim adjustments while also being able to comfortably and consistently track targets. A sensitivity that is too high may lead to over-aiming and lack of control, while a sensitivity that is too low may hinder your ability to react quickly in fast-paced situations. Experimenting with different sensitivities and finding a balance between speed and accuracy is key to determining the perfect sensitivity for you."</v>
+      </c>
+    </row>
+    <row r="26" xml:space="preserve">
+      <c r="A26" t="str">
+        <v>What advice is there for how to fix shaky aim?</v>
+      </c>
+      <c r="B26" t="str" xml:space="preserve">
+        <v xml:space="preserve">"To fix shaky aim, it&amp;apos;s important to focus on improving your wrist and arm stability while aiming. Here are some tips to help you address shaky aim:
+1. **Proper Technique**: Ensure you are using the correct posture and grip on your mouse. Your arm and wrist should be positioned comfortably and ergonomically to reduce strain.
+2. **Adjust Sensitivity**: Experiment with your mouse sensitivity settings to find a balance that works for you. A sensitivity that is too high can lead to overcorrections and shakiness, while a sensitivity that is too low can make it difficult to track targets smoothly.
+3. **Practice Tracking**: Engage in tracking scenarios like Smoothbot, PGTI, or Pasu TI to improve your smooth tracking"</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Does posture, sitting position, and chair height matter in aiming?</v>
+      </c>
+      <c r="B27" t="str">
+        <v>"Yes, posture, sitting position, and chair height are important factors in aiming effectively while gaming. Maintaining good posture can help reduce strain on your body, particularly your back, neck, and shoulders, allowing you to focus better on the game. Sitting position plays a role in how you move your arms and wrists, affecting your aim precision and speed. A chair at the right height ensures your arms are at the proper angle for optimal mouse control, which can improve your aim consistency and comfort during long gaming sessions. It&amp;apos;s recommended to adjust your setup to achieve a posture that is comfortable and conducive to good aim performance."</v>
+      </c>
+    </row>
+    <row r="28" xml:space="preserve">
+      <c r="A28" t="str">
+        <v>What is the best aim trainer software to use and why?</v>
+      </c>
+      <c r="B28" t="str" xml:space="preserve">
+        <v xml:space="preserve">"There are several popular aim trainer software options available, each with its own strengths and features. One of the most renowned aim trainer software is Kovaak&amp;apos;s FPS Aim Trainer. Kovaak&amp;apos;s offers a wide variety of scenarios, including static clicking scenarios like the ones mentioned in the provided text. It provides extensive customization options, allowing players to tailor their training to specific needs. Kovaak&amp;apos;s also has a large and active community, which means there are plenty of resources, guides, and scenarios created by fellow players to help improve your aim.
+Another notable aim trainer is Aim Lab, which is known for its sleek interface and integration with various games like Valorant and Apex Legends. Aim Lab also offers detailed performance tracking and analytics, allowing players to monitor"</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Which aim training software to use?</v>
+      </c>
+      <c r="B29" t="str">
+        <v>"When choosing an aim training software, it ultimately depends on your personal preferences and skill level. If you are willing to invest in your training and want a wide variety of scenarios to choose from, Kovaak&amp;apos;s FPS Aim Trainer is a popular choice. Aimlabs is a great free alternative that is commonly used for competitions and benchmarking. If you are a very high-level player looking for a paid alternative, Aimbeast might be the best option for you. Consider your goals, budget, and desired features to make the best decision for your aim training needs."</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Is it better to use wrist or arm?</v>
+      </c>
+      <c r="B30" t="str">
+        <v>"It is generally recommended to use a combination of both wrist and arm aiming techniques in your gameplay. Utilizing your arm for wider, faster movements and your wrist for smaller, precise adjustments can provide you with a balance of speed and accuracy. By incorporating both techniques, you can adapt to various situations and maximize your aiming potential. Ultimately, finding the right balance between wrist and arm aiming based on your sensitivity and preferences will help you improve your overall aiming skills."</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>When aiming, are you supposed to look at the crosshair or at the target?</v>
+      </c>
+      <c r="B31" t="str">
+        <v>"When aiming, it is generally recommended to focus your gaze on the target rather than the crosshair. By keeping your eyes on the target, you can better predict its movements and make adjustments to your aim accordingly. Your peripheral vision will help you keep track of your crosshair's position in relation to the target. This technique, known as "target focus," allows for smoother and more precise tracking as it helps to improve hand-eye coordination and reaction time. Remember to trust your muscle memory and practice consistently to develop this skill further."</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>What does Viscose say about Raw Accel and mouse acceleration?</v>
+      </c>
+      <c r="B32" t="str">
+        <v>"Viscose initially experienced success with mouse acceleration, but later discovered that it limited her micro-adjustments and masked underlying mechanical issues, particularly in games requiring quick, precise movements. This led her to abandon mouse acceleration in favor of a static sensitivity setting and focused practice to improve her performance significantly. Ultimately, Viscose acknowledges that mouse acceleration had its initial positive impact by motivating her to work on her aim, but she highlights the importance of understanding its limitations and approaching it with realistic expectations."</v>
+      </c>
+    </row>
+    <row r="33" xml:space="preserve">
+      <c r="A33" t="str">
+        <v>What are some good scenarios for CS or VALORANT?</v>
+      </c>
+      <c r="B33" t="str" xml:space="preserve">
+        <v xml:space="preserve">"For improving mouse control and aim in games like VALORANT, there are specific scenarios in aim training platforms like Aim Lab that can be very beneficial. Here are some scenarios that are popular for training in CS:GO and VALORANT:
+1. **Gridshot**: This scenario focuses on flicking accuracy and speed. Targets appear on a grid, and you have to quickly flick and shoot them.
+2. **Spider Shot**: This scenario helps improve your tracking and flicking abilities by shooting moving targets that change direction.
+3. **Strafing FuglaaXY**: This scenario helps with tracking and target acquisition as the targets move in erratic patterns.
+4. **Microshot Speed**: This scenario is great for improving your click-timing and"</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Does Voltaic manage an active esports team within aim training?</v>
+      </c>
+      <c r="B34" t="str">
+        <v>"Voltaic Systems is known for providing high-quality aim training scenarios and routines for esports players, but they do not manage an active esports team themselves. Their focus is on creating tools and resources to help players improve their aim, reflexes, and overall performance in games like Overwatch. Players and teams can utilize Voltaic's training routines to enhance their skills and compete at a higher level in the esports scene."</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H34"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed off by 1 formatting bug in ChatData.xlsx
</commit_message>
<xml_diff>
--- a/ChatData.xlsx
+++ b/ChatData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parsp\OneDrive\Desktop\All\Online\PersonalProject\AimJourney\aimjourney\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE02C806-7B55-419F-B3F2-3AAF9DA23811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEAE0CA-E0CE-4444-9FA6-E6F482D562D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>